<commit_message>
tweaked thresholds again, weak threshold seemingly not working
</commit_message>
<xml_diff>
--- a/TestFiles/AIMData.xlsx
+++ b/TestFiles/AIMData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339693D2-23BA-4EE7-B327-B63C1679F7A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6789BED1-4562-444F-8DC6-CAE8F3B3787F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4152" yWindow="1860" windowWidth="17280" windowHeight="8964" xr2:uid="{E013ABEC-2059-4040-973C-94727C750888}"/>
+    <workbookView xWindow="29190" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{E013ABEC-2059-4040-973C-94727C750888}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -520,17 +520,17 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.77734375" customWidth="1"/>
+    <col min="1" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>20191011</v>
       </c>
@@ -559,7 +559,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>20191594</v>
       </c>
@@ -574,7 +574,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>20190680</v>
       </c>
@@ -589,7 +589,7 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>20191062</v>
       </c>
@@ -604,7 +604,7 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>20191359</v>
       </c>
@@ -619,7 +619,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>20190318</v>
       </c>
@@ -634,7 +634,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>20190950</v>
       </c>
@@ -649,7 +649,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>20190962</v>
       </c>
@@ -664,7 +664,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>20190964</v>
       </c>
@@ -679,7 +679,7 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>20190977</v>
       </c>
@@ -694,7 +694,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>20191095</v>
       </c>
@@ -709,7 +709,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>20182259</v>
       </c>
@@ -724,7 +724,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>20182704</v>
       </c>
@@ -739,7 +739,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>20190021</v>
       </c>
@@ -754,7 +754,7 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>20190096</v>
       </c>
@@ -769,7 +769,7 @@
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>20182625</v>
       </c>
@@ -784,7 +784,7 @@
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>20190248</v>
       </c>
@@ -799,7 +799,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>20190844</v>
       </c>
@@ -814,7 +814,7 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>20191362</v>
       </c>
@@ -829,7 +829,7 @@
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20191084</v>
       </c>
@@ -844,15 +844,15 @@
       </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New version of HATCo program
</commit_message>
<xml_diff>
--- a/TestFiles/AIMData.xlsx
+++ b/TestFiles/AIMData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\Source\Repos\BuschEric97\HatcoFilesClosedDeterminer\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6789BED1-4562-444F-8DC6-CAE8F3B3787F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6E6553-20AD-4957-8DC8-0D6EF6AC2216}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{E013ABEC-2059-4040-973C-94727C750888}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E013ABEC-2059-4040-973C-94727C750888}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>File Number</t>
   </si>
@@ -163,6 +163,69 @@
   </si>
   <si>
     <t>Jody Harland; Rebecca Harland</t>
+  </si>
+  <si>
+    <t>Escrow Officer</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>test6</t>
+  </si>
+  <si>
+    <t>test7</t>
+  </si>
+  <si>
+    <t>test8</t>
+  </si>
+  <si>
+    <t>test9</t>
+  </si>
+  <si>
+    <t>test10</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>test12</t>
+  </si>
+  <si>
+    <t>test13</t>
+  </si>
+  <si>
+    <t>test14</t>
+  </si>
+  <si>
+    <t>test15</t>
+  </si>
+  <si>
+    <t>test16</t>
+  </si>
+  <si>
+    <t>test17</t>
+  </si>
+  <si>
+    <t>test18</t>
+  </si>
+  <si>
+    <t>test19</t>
+  </si>
+  <si>
+    <t>test20</t>
   </si>
 </sst>
 </file>
@@ -520,7 +583,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,6 +591,7 @@
     <col min="1" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -543,6 +607,9 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -557,7 +624,9 @@
       <c r="D2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -572,7 +641,9 @@
       <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -587,7 +658,9 @@
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -602,7 +675,9 @@
       <c r="D5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -617,7 +692,9 @@
       <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -632,7 +709,9 @@
       <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -647,7 +726,9 @@
       <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -662,7 +743,9 @@
       <c r="D9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -677,7 +760,9 @@
       <c r="D10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -692,7 +777,9 @@
       <c r="D11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -707,7 +794,9 @@
       <c r="D12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -722,7 +811,9 @@
       <c r="D13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -737,7 +828,9 @@
       <c r="D14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -752,7 +845,9 @@
       <c r="D15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -767,7 +862,9 @@
       <c r="D16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -782,7 +879,9 @@
       <c r="D17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -797,7 +896,9 @@
       <c r="D18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -812,7 +913,9 @@
       <c r="D19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -827,7 +930,9 @@
       <c r="D20" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -842,7 +947,9 @@
       <c r="D21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>

</xml_diff>